<commit_message>
Commmited after changing some changes
</commit_message>
<xml_diff>
--- a/TestDataFiles/contacts.xlsx
+++ b/TestDataFiles/contacts.xlsx
@@ -356,7 +356,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -369,7 +369,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>8634503046</v>
+        <v>8634502057</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -377,7 +377,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>8634503047</v>
+        <v>8634502058</v>
       </c>
     </row>
   </sheetData>

</xml_diff>